<commit_message>
Fix dashboard filtering and data reset functionality
Updates the data filtering logic for the dashboard to correctly use date range parameters. Implements the data reset functionality by deleting and recreating the shop_data.xlsx file. Addresses a loading error in the "Data Management" section, likely related to the data reset issue.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 29d07fb8-b988-4773-b40e-6f50fcdf7033
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/2b399e3d-ac6e-437b-bd36-8db339239647/29d07fb8-b988-4773-b40e-6f50fcdf7033/NE0ysOL
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -445,197 +445,121 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>prod-001</v>
+        <v>prod-002</v>
       </c>
       <c r="B2" t="str">
-        <v>iPhone 14 Pro</v>
+        <v>Samsung Galaxy Watch 5</v>
       </c>
       <c r="C2" t="str">
-        <v>Latest Apple iPhone with advanced camera system</v>
+        <v>Advanced smartwatch with health monitoring</v>
       </c>
       <c r="D2">
-        <v>99999</v>
+        <v>25999</v>
       </c>
       <c r="E2">
-        <v>75000</v>
+        <v>20000</v>
       </c>
       <c r="F2" t="str">
         <v>Electronics</v>
       </c>
       <c r="G2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2" t="str">
-        <v>Apple India</v>
+        <v>Samsung Electronics</v>
       </c>
       <c r="J2" t="str">
-        <v>APPLE-IP14PRO-128</v>
+        <v>SAMSUNG-GW5-44MM</v>
       </c>
       <c r="K2">
-        <v>45292</v>
-      </c>
-      <c r="L2" t="str">
-        <v>2025-09-03T13:19:39.402Z</v>
+        <v>45293</v>
+      </c>
+      <c r="L2">
+        <v>45301</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>prod-002</v>
+        <v>prod-003</v>
       </c>
       <c r="B3" t="str">
-        <v>Samsung Galaxy Watch 5</v>
+        <v>MacBook Air M2</v>
       </c>
       <c r="C3" t="str">
-        <v>Advanced smartwatch with health monitoring</v>
+        <v>Lightweight laptop with M2 chip</v>
       </c>
       <c r="D3">
-        <v>25999</v>
+        <v>119999</v>
       </c>
       <c r="E3">
-        <v>20000</v>
+        <v>95000</v>
       </c>
       <c r="F3" t="str">
-        <v>Electronics</v>
+        <v>Computers</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" t="str">
-        <v>Samsung Electronics</v>
+        <v>Apple India</v>
       </c>
       <c r="J3" t="str">
-        <v>SAMSUNG-GW5-44MM</v>
+        <v>APPLE-MBA-M2-256</v>
       </c>
       <c r="K3">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="L3">
-        <v>45301</v>
+        <v>45303</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>prod-003</v>
+        <v>prod-004</v>
       </c>
       <c r="B4" t="str">
-        <v>MacBook Air M2</v>
+        <v>AirPods Pro</v>
       </c>
       <c r="C4" t="str">
-        <v>Lightweight laptop with M2 chip</v>
+        <v>Wireless earbuds with active noise cancellation</v>
       </c>
       <c r="D4">
-        <v>119999</v>
+        <v>24900</v>
       </c>
       <c r="E4">
-        <v>95000</v>
+        <v>18000</v>
       </c>
       <c r="F4" t="str">
-        <v>Computers</v>
+        <v>Audio</v>
       </c>
       <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4">
         <v>5</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
       </c>
       <c r="I4" t="str">
         <v>Apple India</v>
       </c>
       <c r="J4" t="str">
-        <v>APPLE-MBA-M2-256</v>
+        <v>APPLE-APP-2ND-GEN</v>
       </c>
       <c r="K4">
-        <v>45294</v>
-      </c>
-      <c r="L4">
-        <v>45303</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>prod-004</v>
-      </c>
-      <c r="B5" t="str">
-        <v>AirPods Pro</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Wireless earbuds with active noise cancellation</v>
-      </c>
-      <c r="D5">
-        <v>24900</v>
-      </c>
-      <c r="E5">
-        <v>18000</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Audio</v>
-      </c>
-      <c r="G5">
-        <v>200</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Apple India</v>
-      </c>
-      <c r="J5" t="str">
-        <v>APPLE-APP-2ND-GEN</v>
-      </c>
-      <c r="K5">
         <v>45295</v>
       </c>
-      <c r="L5" t="str">
+      <c r="L4" t="str">
         <v>2025-09-08T11:06:46.594Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>prod-005</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Dell XPS 13</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Premium ultrabook for professionals</v>
-      </c>
-      <c r="D6">
-        <v>95999</v>
-      </c>
-      <c r="E6">
-        <v>80000</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Computers</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Dell Technologies</v>
-      </c>
-      <c r="J6" t="str">
-        <v>DELL-XPS13-I7-512</v>
-      </c>
-      <c r="K6">
-        <v>45296</v>
-      </c>
-      <c r="L6">
-        <v>45305</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update shop data with new information
Updates the shop data file with new product or pricing information.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 29d07fb8-b988-4773-b40e-6f50fcdf7033
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/2b399e3d-ac6e-437b-bd36-8db339239647/29d07fb8-b988-4773-b40e-6f50fcdf7033/NE0ysOL
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -402,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -454,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -506,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Automate desktop application builds and deployment using GitHub Actions
Introduces automated build workflows for desktop applications using GitHub Actions, addressing local build environment issues like disk quotas and file locking. Adds new workflow files for automatic and manual builds (.yml), updates package.json with `electronRebuild` setting, and includes a FUNDING.yml file. Also updates a markdown guide with build process details.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 29d07fb8-b988-4773-b40e-6f50fcdf7033
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/2b399e3d-ac6e-437b-bd36-8db339239647/29d07fb8-b988-4773-b40e-6f50fcdf7033/NE0ysOL
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -400,104 +400,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>cost_price</v>
+      </c>
+      <c r="E1" t="str">
+        <v>category</v>
+      </c>
+      <c r="F1" t="str">
+        <v>stock</v>
+      </c>
+      <c r="G1" t="str">
+        <v>min_stock</v>
+      </c>
+      <c r="H1" t="str">
+        <v>supplier</v>
+      </c>
+      <c r="I1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="J1" t="str">
         <v>id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>description</v>
-      </c>
-      <c r="D1" t="str">
-        <v>price</v>
-      </c>
-      <c r="E1" t="str">
-        <v>cost_price</v>
-      </c>
-      <c r="F1" t="str">
-        <v>category</v>
-      </c>
-      <c r="G1" t="str">
-        <v>stock</v>
-      </c>
-      <c r="H1" t="str">
-        <v>min_stock</v>
-      </c>
-      <c r="I1" t="str">
-        <v>supplier</v>
-      </c>
-      <c r="J1" t="str">
-        <v>sku</v>
       </c>
       <c r="K1" t="str">
         <v>created_date</v>
       </c>
       <c r="L1" t="str">
         <v>last_updated</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>amul</v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v>100</v>
+      </c>
+      <c r="D2" t="str">
+        <v>50</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Food</v>
+      </c>
+      <c r="F2">
+        <v>80</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v>285f3854-cbf2-4ba5-b477-5cda3035ab2d</v>
+      </c>
+      <c r="K2" t="str">
+        <v>2025-09-12T12:06:21.787Z</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2025-09-12T12:06:48.292Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>product_id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>quantity</v>
+      </c>
+      <c r="C1" t="str">
+        <v>unit_price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>customer_name</v>
+      </c>
+      <c r="E1" t="str">
+        <v>payment_method</v>
+      </c>
+      <c r="F1" t="str">
+        <v>cashier</v>
+      </c>
+      <c r="G1" t="str">
+        <v>notes</v>
+      </c>
+      <c r="H1" t="str">
         <v>id</v>
       </c>
-      <c r="B1" t="str">
-        <v>product_id</v>
-      </c>
-      <c r="C1" t="str">
+      <c r="I1" t="str">
         <v>product_name</v>
       </c>
-      <c r="D1" t="str">
-        <v>quantity</v>
-      </c>
-      <c r="E1" t="str">
-        <v>unit_price</v>
-      </c>
-      <c r="F1" t="str">
+      <c r="J1" t="str">
         <v>total_amount</v>
       </c>
-      <c r="G1" t="str">
+      <c r="K1" t="str">
         <v>profit</v>
       </c>
-      <c r="H1" t="str">
-        <v>customer_name</v>
-      </c>
-      <c r="I1" t="str">
-        <v>payment_method</v>
-      </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>sale_date</v>
       </c>
-      <c r="K1" t="str">
-        <v>cashier</v>
-      </c>
-      <c r="L1" t="str">
-        <v>notes</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>285f3854-cbf2-4ba5-b477-5cda3035ab2d</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="str">
+        <v>100</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Zeeshan</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v>937b64d0-f047-42cc-b7ea-14a294d8ed1c</v>
+      </c>
+      <c r="I2" t="str">
+        <v>amul</v>
+      </c>
+      <c r="J2" t="str">
+        <v>2000</v>
+      </c>
+      <c r="K2" t="str">
+        <v>1000</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2025-09-12T12:06:48.282Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add initial shop data and backup for the dataset
Add `shop_data.xlsx` to the data directory and create a backup of `shop_data.xlsx`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: cd8208a5-89b9-41aa-9133-76bfd169e5f0
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/910a9461-2a06-4903-a94b-1a2faea688f1/cd8208a5-89b9-41aa-9133-76bfd169e5f0/tdnbheC
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -400,180 +400,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>description</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>price</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>cost_price</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>category</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>stock</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>min_stock</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>supplier</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>sku</v>
-      </c>
-      <c r="J1" t="str">
-        <v>id</v>
       </c>
       <c r="K1" t="str">
         <v>created_date</v>
       </c>
       <c r="L1" t="str">
         <v>last_updated</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>amul</v>
-      </c>
-      <c r="B2" t="str">
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <v>100</v>
-      </c>
-      <c r="D2" t="str">
-        <v>50</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Food</v>
-      </c>
-      <c r="F2">
-        <v>80</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="str">
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <v>285f3854-cbf2-4ba5-b477-5cda3035ab2d</v>
-      </c>
-      <c r="K2" t="str">
-        <v>2025-09-12T12:06:21.787Z</v>
-      </c>
-      <c r="L2" t="str">
-        <v>2025-09-12T12:06:48.292Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
         <v>product_id</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
+        <v>product_name</v>
+      </c>
+      <c r="D1" t="str">
         <v>quantity</v>
       </c>
-      <c r="C1" t="str">
+      <c r="E1" t="str">
         <v>unit_price</v>
       </c>
-      <c r="D1" t="str">
+      <c r="F1" t="str">
+        <v>total_amount</v>
+      </c>
+      <c r="G1" t="str">
+        <v>profit</v>
+      </c>
+      <c r="H1" t="str">
         <v>customer_name</v>
       </c>
-      <c r="E1" t="str">
+      <c r="I1" t="str">
         <v>payment_method</v>
       </c>
-      <c r="F1" t="str">
+      <c r="J1" t="str">
+        <v>sale_date</v>
+      </c>
+      <c r="K1" t="str">
         <v>cashier</v>
       </c>
-      <c r="G1" t="str">
+      <c r="L1" t="str">
         <v>notes</v>
-      </c>
-      <c r="H1" t="str">
-        <v>id</v>
-      </c>
-      <c r="I1" t="str">
-        <v>product_name</v>
-      </c>
-      <c r="J1" t="str">
-        <v>total_amount</v>
-      </c>
-      <c r="K1" t="str">
-        <v>profit</v>
-      </c>
-      <c r="L1" t="str">
-        <v>sale_date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>285f3854-cbf2-4ba5-b477-5cda3035ab2d</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="str">
-        <v>100</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Zeeshan</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Admin</v>
-      </c>
-      <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v>937b64d0-f047-42cc-b7ea-14a294d8ed1c</v>
-      </c>
-      <c r="I2" t="str">
-        <v>amul</v>
-      </c>
-      <c r="J2" t="str">
-        <v>2000</v>
-      </c>
-      <c r="K2" t="str">
-        <v>1000</v>
-      </c>
-      <c r="L2" t="str">
-        <v>2025-09-12T12:06:48.282Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update application to use a custom logo and ensure accurate date ranges
Update the application's icon files and ensure end dates are set to the last millisecond of the day for accurate data fetching.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: cc5b71e4-8635-4a41-a1bc-5434bc891a02
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/932172d4-088a-4428-803b-ea21e9ddc05b/cc5b71e4-8635-4a41-a1bc-5434bc891a02/WxNtjR3
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -400,147 +400,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>cost_price</v>
+      </c>
+      <c r="E1" t="str">
+        <v>category</v>
+      </c>
+      <c r="F1" t="str">
+        <v>stock</v>
+      </c>
+      <c r="G1" t="str">
+        <v>min_stock</v>
+      </c>
+      <c r="H1" t="str">
+        <v>supplier</v>
+      </c>
+      <c r="I1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="J1" t="str">
         <v>id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>description</v>
-      </c>
-      <c r="D1" t="str">
-        <v>price</v>
-      </c>
-      <c r="E1" t="str">
-        <v>cost_price</v>
-      </c>
-      <c r="F1" t="str">
-        <v>category</v>
-      </c>
-      <c r="G1" t="str">
-        <v>stock</v>
-      </c>
-      <c r="H1" t="str">
-        <v>min_stock</v>
-      </c>
-      <c r="I1" t="str">
-        <v>supplier</v>
-      </c>
-      <c r="J1" t="str">
-        <v>sku</v>
       </c>
       <c r="K1" t="str">
         <v>created_date</v>
       </c>
       <c r="L1" t="str">
         <v>last_updated</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Amul Butter (500g)</v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="str">
+        <v>10</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Clothing</v>
+      </c>
+      <c r="F2">
+        <v>450</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v>79bf20ff-9535-45ea-9dcd-a9596ae5258a</v>
+      </c>
+      <c r="K2" t="str">
+        <v>2025-09-23T11:20:28.437Z</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2025-09-23T11:20:38.822Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>product_id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>quantity</v>
+      </c>
+      <c r="C1" t="str">
+        <v>unit_price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>customer_name</v>
+      </c>
+      <c r="E1" t="str">
+        <v>payment_method</v>
+      </c>
+      <c r="F1" t="str">
+        <v>cashier</v>
+      </c>
+      <c r="G1" t="str">
+        <v>notes</v>
+      </c>
+      <c r="H1" t="str">
         <v>id</v>
       </c>
-      <c r="B1" t="str">
-        <v>product_id</v>
-      </c>
-      <c r="C1" t="str">
+      <c r="I1" t="str">
         <v>product_name</v>
       </c>
-      <c r="D1" t="str">
-        <v>quantity</v>
-      </c>
-      <c r="E1" t="str">
-        <v>unit_price</v>
-      </c>
-      <c r="F1" t="str">
+      <c r="J1" t="str">
         <v>total_amount</v>
       </c>
-      <c r="G1" t="str">
+      <c r="K1" t="str">
         <v>profit</v>
       </c>
-      <c r="H1" t="str">
-        <v>customer_name</v>
-      </c>
-      <c r="I1" t="str">
-        <v>payment_method</v>
-      </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>sale_date</v>
       </c>
-      <c r="K1" t="str">
-        <v>cashier</v>
-      </c>
-      <c r="L1" t="str">
-        <v>notes</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>79bf20ff-9535-45ea-9dcd-a9596ae5258a</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="str">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v>cae2620a-9922-4239-8ac5-97c254e4019b</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Amul Butter (500g)</v>
+      </c>
+      <c r="J2" t="str">
+        <v>50000</v>
+      </c>
+      <c r="K2" t="str">
+        <v>49500</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2025-09-23T11:20:38.815Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>category</v>
+      </c>
+      <c r="B1" t="str">
+        <v>description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>amount</v>
+      </c>
+      <c r="D1" t="str">
+        <v>payment_method</v>
+      </c>
+      <c r="E1" t="str">
+        <v>vendor</v>
+      </c>
+      <c r="F1" t="str">
+        <v>notes</v>
+      </c>
+      <c r="G1" t="str">
         <v>id</v>
       </c>
-      <c r="B1" t="str">
-        <v>category</v>
-      </c>
-      <c r="C1" t="str">
-        <v>description</v>
-      </c>
-      <c r="D1" t="str">
-        <v>amount</v>
-      </c>
-      <c r="E1" t="str">
-        <v>payment_method</v>
-      </c>
-      <c r="F1" t="str">
-        <v>vendor</v>
-      </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>expense_date</v>
       </c>
-      <c r="H1" t="str">
-        <v>receipt_number</v>
-      </c>
-      <c r="I1" t="str">
-        <v>notes</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Rent</v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v>5000</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v>ed6c6149-eea7-457f-95a8-eb25cdf5b985</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2025-09-23T11:26:47.809Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Checkpoint before assistant change: Fix calculation of net profit by correctly subtracting expenses
Update shop_data.xlsx to ensure accurate net profit calculation (Total Revenue - Total Expenses).

Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -400,246 +400,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>description</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>price</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>cost_price</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>category</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>stock</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>min_stock</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>supplier</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>sku</v>
-      </c>
-      <c r="J1" t="str">
-        <v>id</v>
       </c>
       <c r="K1" t="str">
         <v>created_date</v>
       </c>
       <c r="L1" t="str">
         <v>last_updated</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Amul Butter (500g)</v>
-      </c>
-      <c r="B2" t="str">
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <v>1000</v>
-      </c>
-      <c r="D2" t="str">
-        <v>10</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Clothing</v>
-      </c>
-      <c r="F2">
-        <v>450</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="str">
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <v>79bf20ff-9535-45ea-9dcd-a9596ae5258a</v>
-      </c>
-      <c r="K2" t="str">
-        <v>2025-09-23T11:20:28.437Z</v>
-      </c>
-      <c r="L2" t="str">
-        <v>2025-09-23T11:20:38.822Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
         <v>product_id</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
+        <v>product_name</v>
+      </c>
+      <c r="D1" t="str">
         <v>quantity</v>
       </c>
-      <c r="C1" t="str">
+      <c r="E1" t="str">
         <v>unit_price</v>
       </c>
-      <c r="D1" t="str">
+      <c r="F1" t="str">
+        <v>total_amount</v>
+      </c>
+      <c r="G1" t="str">
+        <v>profit</v>
+      </c>
+      <c r="H1" t="str">
         <v>customer_name</v>
       </c>
-      <c r="E1" t="str">
+      <c r="I1" t="str">
         <v>payment_method</v>
       </c>
-      <c r="F1" t="str">
+      <c r="J1" t="str">
+        <v>sale_date</v>
+      </c>
+      <c r="K1" t="str">
         <v>cashier</v>
       </c>
-      <c r="G1" t="str">
+      <c r="L1" t="str">
         <v>notes</v>
-      </c>
-      <c r="H1" t="str">
-        <v>id</v>
-      </c>
-      <c r="I1" t="str">
-        <v>product_name</v>
-      </c>
-      <c r="J1" t="str">
-        <v>total_amount</v>
-      </c>
-      <c r="K1" t="str">
-        <v>profit</v>
-      </c>
-      <c r="L1" t="str">
-        <v>sale_date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>79bf20ff-9535-45ea-9dcd-a9596ae5258a</v>
-      </c>
-      <c r="B2">
-        <v>50</v>
-      </c>
-      <c r="C2" t="str">
-        <v>1000</v>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Admin</v>
-      </c>
-      <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v>cae2620a-9922-4239-8ac5-97c254e4019b</v>
-      </c>
-      <c r="I2" t="str">
-        <v>Amul Butter (500g)</v>
-      </c>
-      <c r="J2" t="str">
-        <v>50000</v>
-      </c>
-      <c r="K2" t="str">
-        <v>49500</v>
-      </c>
-      <c r="L2" t="str">
-        <v>2025-09-23T11:20:38.815Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
         <v>category</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>description</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>amount</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>payment_method</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>vendor</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
+        <v>expense_date</v>
+      </c>
+      <c r="H1" t="str">
+        <v>receipt_number</v>
+      </c>
+      <c r="I1" t="str">
         <v>notes</v>
-      </c>
-      <c r="G1" t="str">
-        <v>id</v>
-      </c>
-      <c r="H1" t="str">
-        <v>expense_date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Rent</v>
-      </c>
-      <c r="B2" t="str">
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <v>5000</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v>ed6c6149-eea7-457f-95a8-eb25cdf5b985</v>
-      </c>
-      <c r="H2" t="str">
-        <v>2025-09-23T11:26:47.809Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update shop branding and receipt printing functionality
Replaces logos across the application with a new one and refactors the receipt printing component to support thermal printers with improved styling, layout, and automatic print dialog integration. Also updates KPI calculations to include net profit and net margin.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 77c3528f-62ac-4822-a3b0-33496d116cac
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0f67d2ec-15fd-4721-bd99-7c537bf3758d/77c3528f-62ac-4822-a3b0-33496d116cac/qHQ3QVq
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -400,147 +400,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>cost_price</v>
+      </c>
+      <c r="E1" t="str">
+        <v>category</v>
+      </c>
+      <c r="F1" t="str">
+        <v>stock</v>
+      </c>
+      <c r="G1" t="str">
+        <v>min_stock</v>
+      </c>
+      <c r="H1" t="str">
+        <v>supplier</v>
+      </c>
+      <c r="I1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="J1" t="str">
         <v>id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>description</v>
-      </c>
-      <c r="D1" t="str">
-        <v>price</v>
-      </c>
-      <c r="E1" t="str">
-        <v>cost_price</v>
-      </c>
-      <c r="F1" t="str">
-        <v>category</v>
-      </c>
-      <c r="G1" t="str">
-        <v>stock</v>
-      </c>
-      <c r="H1" t="str">
-        <v>min_stock</v>
-      </c>
-      <c r="I1" t="str">
-        <v>supplier</v>
-      </c>
-      <c r="J1" t="str">
-        <v>sku</v>
       </c>
       <c r="K1" t="str">
         <v>created_date</v>
       </c>
       <c r="L1" t="str">
         <v>last_updated</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Amul Butter (500g)</v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Food</v>
+      </c>
+      <c r="F2">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v>07291cea-a90f-4352-b915-1121e63dcb59</v>
+      </c>
+      <c r="K2" t="str">
+        <v>2025-09-23T12:50:58.115Z</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2025-09-23T12:51:14.513Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>product_id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>quantity</v>
+      </c>
+      <c r="C1" t="str">
+        <v>unit_price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>customer_name</v>
+      </c>
+      <c r="E1" t="str">
+        <v>payment_method</v>
+      </c>
+      <c r="F1" t="str">
+        <v>cashier</v>
+      </c>
+      <c r="G1" t="str">
+        <v>notes</v>
+      </c>
+      <c r="H1" t="str">
         <v>id</v>
       </c>
-      <c r="B1" t="str">
-        <v>product_id</v>
-      </c>
-      <c r="C1" t="str">
+      <c r="I1" t="str">
         <v>product_name</v>
       </c>
-      <c r="D1" t="str">
-        <v>quantity</v>
-      </c>
-      <c r="E1" t="str">
-        <v>unit_price</v>
-      </c>
-      <c r="F1" t="str">
+      <c r="J1" t="str">
         <v>total_amount</v>
       </c>
-      <c r="G1" t="str">
+      <c r="K1" t="str">
         <v>profit</v>
       </c>
-      <c r="H1" t="str">
-        <v>customer_name</v>
-      </c>
-      <c r="I1" t="str">
-        <v>payment_method</v>
-      </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>sale_date</v>
       </c>
-      <c r="K1" t="str">
-        <v>cashier</v>
-      </c>
-      <c r="L1" t="str">
-        <v>notes</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>07291cea-a90f-4352-b915-1121e63dcb59</v>
+      </c>
+      <c r="B2">
+        <v>71</v>
+      </c>
+      <c r="C2" t="str">
+        <v>500</v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v>9cbf4f85-2a79-4a90-8951-8c7ed4927e8d</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Amul Butter (500g)</v>
+      </c>
+      <c r="J2" t="str">
+        <v>35500</v>
+      </c>
+      <c r="K2" t="str">
+        <v>28400</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2025-09-23T12:51:14.506Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>category</v>
+      </c>
+      <c r="B1" t="str">
+        <v>description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>amount</v>
+      </c>
+      <c r="D1" t="str">
+        <v>payment_method</v>
+      </c>
+      <c r="E1" t="str">
+        <v>vendor</v>
+      </c>
+      <c r="F1" t="str">
+        <v>notes</v>
+      </c>
+      <c r="G1" t="str">
         <v>id</v>
       </c>
-      <c r="B1" t="str">
-        <v>category</v>
-      </c>
-      <c r="C1" t="str">
-        <v>description</v>
-      </c>
-      <c r="D1" t="str">
-        <v>amount</v>
-      </c>
-      <c r="E1" t="str">
-        <v>payment_method</v>
-      </c>
-      <c r="F1" t="str">
-        <v>vendor</v>
-      </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>expense_date</v>
       </c>
-      <c r="H1" t="str">
-        <v>receipt_number</v>
-      </c>
-      <c r="I1" t="str">
-        <v>notes</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Utilities</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Random</v>
+      </c>
+      <c r="C2" t="str">
+        <v>5000</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v>0f1d1996-63c0-461d-b044-35309c9cda10</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2025-09-23T12:51:31.350Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update shop data with new product information
Updated `data/shop_data.xlsx` to include new product details.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 77c3528f-62ac-4822-a3b0-33496d116cac
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0f67d2ec-15fd-4721-bd99-7c537bf3758d/77c3528f-62ac-4822-a3b0-33496d116cac/qHQ3QVq
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -460,7 +460,7 @@
         <v>Food</v>
       </c>
       <c r="F2">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -478,7 +478,7 @@
         <v>2025-09-23T12:50:58.115Z</v>
       </c>
       <c r="L2" t="str">
-        <v>2025-09-23T12:51:14.513Z</v>
+        <v>2025-09-23T13:02:08.605Z</v>
       </c>
     </row>
   </sheetData>
@@ -490,7 +490,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -571,9 +571,47 @@
         <v>2025-09-23T12:51:14.506Z</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>07291cea-a90f-4352-b915-1121e63dcb59</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="str">
+        <v>500</v>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v>e66c2199-14fc-46af-b2ee-ed7812584635</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Amul Butter (500g)</v>
+      </c>
+      <c r="J3" t="str">
+        <v>5000</v>
+      </c>
+      <c r="K3" t="str">
+        <v>4000</v>
+      </c>
+      <c r="L3" t="str">
+        <v>2025-09-23T13:02:08.595Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Checkpoint before assistant change: Update shop data with the latest information
Updated the shop_data.xlsx file with new entries.

Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -460,7 +460,7 @@
         <v>Food</v>
       </c>
       <c r="F2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -478,7 +478,7 @@
         <v>2025-09-23T12:50:58.115Z</v>
       </c>
       <c r="L2" t="str">
-        <v>2025-09-23T13:02:08.605Z</v>
+        <v>2025-09-23T13:05:26.195Z</v>
       </c>
     </row>
   </sheetData>
@@ -490,7 +490,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -609,9 +609,47 @@
         <v>2025-09-23T13:02:08.595Z</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>07291cea-a90f-4352-b915-1121e63dcb59</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>500</v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v>15ca83ea-a74c-421a-911c-b93c602bde13</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Amul Butter (500g)</v>
+      </c>
+      <c r="J4" t="str">
+        <v>500</v>
+      </c>
+      <c r="K4" t="str">
+        <v>400</v>
+      </c>
+      <c r="L4" t="str">
+        <v>2025-09-23T13:05:26.171Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>